<commit_message>
fixed main program to store results better fixed main program so it won't regenerate data each iteration fixed matlab files to go with main program fixes fixed example cpt ranges file to be ANDs
</commit_message>
<xml_diff>
--- a/Example/CPT_Table_Ranges _WithHeaders.xlsx
+++ b/Example/CPT_Table_Ranges _WithHeaders.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="17235" windowHeight="10290"/>
+    <workbookView xWindow="240" yWindow="180" windowWidth="17235" windowHeight="10230"/>
   </bookViews>
   <sheets>
     <sheet name="CPT_Table_Ranges _WithHeaders" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>.5-.9</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Parents</t>
+  </si>
+  <si>
+    <t>.3-.7</t>
   </si>
 </sst>
 </file>
@@ -893,15 +896,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
@@ -909,8 +912,15 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>0</v>
       </c>
@@ -926,8 +936,23 @@
       <c r="G2">
         <v>4</v>
       </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -949,8 +974,29 @@
       <c r="G3" t="s">
         <v>1</v>
       </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -969,8 +1015,26 @@
       <c r="G4" t="s">
         <v>1</v>
       </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -989,8 +1053,26 @@
       <c r="G5" t="s">
         <v>1</v>
       </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -1009,8 +1091,26 @@
       <c r="G6" t="s">
         <v>1</v>
       </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1029,10 +1129,29 @@
       <c r="G7" t="s">
         <v>13</v>
       </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:G1"/>
+    <mergeCell ref="M1:Q1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>